<commit_message>
Modificações - gráficos para paper
</commit_message>
<xml_diff>
--- a/Parâmetros.xlsx
+++ b/Parâmetros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E7994B-2036-4878-8ED2-44635B9DE836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6818A84-CE4F-4CD6-94E3-855686D6FF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="15">
         <v>0.1</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="15">
-        <v>0.2828</v>
+        <v>0.2</v>
       </c>
       <c r="L2" s="10">
         <v>2</v>

</xml_diff>

<commit_message>
Modelos para o artigo
</commit_message>
<xml_diff>
--- a/Parâmetros.xlsx
+++ b/Parâmetros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0894978-F2E7-46F0-856C-CE41B1F42440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E5F52B-FC39-4328-8D8A-A9ACC8BD7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
+    <workbookView xWindow="14655" yWindow="1050" windowWidth="22155" windowHeight="13545" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -386,7 +386,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64130676-9D84-4B43-9CC6-731DFC23A473}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" s="15">
         <v>0.1</v>
@@ -855,7 +855,7 @@
         <v>3.5857199999999998</v>
       </c>
       <c r="R2" s="16">
-        <v>85</v>
+        <v>83.178899680000001</v>
       </c>
       <c r="S2" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
Correção da impressão das cores nas curvas de luz
As cores do espectro estavam invertidas
</commit_message>
<xml_diff>
--- a/Parâmetros.xlsx
+++ b/Parâmetros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E5F52B-FC39-4328-8D8A-A9ACC8BD7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E34611D-127C-4645-BF1D-CF49313E8128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14655" yWindow="1050" windowWidth="22155" windowHeight="13545" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -386,7 +386,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -709,7 +709,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,7 @@
         <v>3.5857199999999998</v>
       </c>
       <c r="R2" s="16">
-        <v>83.178899680000001</v>
+        <v>85</v>
       </c>
       <c r="S2" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
Simulações para 55Cnc e
</commit_message>
<xml_diff>
--- a/Parâmetros.xlsx
+++ b/Parâmetros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\StarsAndExoplanets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4A1D6-923B-471E-990D-C1E083F9164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463D3937-F8BB-4869-9F31-6702AB35E772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{135A0AB5-F6C2-44B6-B5E2-B976BC3DCBD2}"/>
   </bookViews>
@@ -162,15 +162,16 @@
     <t>object</t>
   </si>
   <si>
-    <t>GJ9827d</t>
+    <t>55Cnc_e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -366,7 +367,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -436,6 +437,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -763,7 +767,7 @@
   <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +879,7 @@
         <v>2050</v>
       </c>
       <c r="F2" s="8">
-        <v>0.60199999999999998</v>
+        <v>0.95</v>
       </c>
       <c r="G2" s="8">
         <v>0</v>
@@ -884,37 +888,37 @@
         <v>0</v>
       </c>
       <c r="I2" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="18">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="18">
         <v>0</v>
       </c>
       <c r="L2" s="18">
-        <v>0.28284271249999998</v>
+        <v>0.2</v>
       </c>
       <c r="M2" s="19">
         <v>2</v>
       </c>
       <c r="N2" s="19">
-        <v>5.5899999999999998E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="O2" s="20">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="P2" s="20">
-        <v>0.182</v>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="P2" s="24">
+        <v>0.16192000000000001</v>
       </c>
       <c r="Q2" s="20">
-        <v>7.3899999999999999E-3</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="R2" s="20">
-        <v>6.2014189999999996</v>
-      </c>
-      <c r="S2" s="24">
-        <v>89.017641452899696</v>
+        <v>0.73653900000000005</v>
+      </c>
+      <c r="S2" s="25">
+        <v>74.387874007958203</v>
       </c>
       <c r="T2" s="21">
         <v>0</v>
@@ -933,9 +937,6 @@
       </c>
       <c r="Y2" s="23">
         <v>0</v>
-      </c>
-      <c r="AB2" s="18">
-        <v>0.28284271249999998</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -960,6 +961,9 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
+      <c r="AB3" s="18">
+        <v>0.28284271249999998</v>
+      </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>

</xml_diff>